<commit_message>
Refactor: Arrumando qual coluna pegar da tabela de contratante e aluno e sempre colocando o relatório de NPS 10 linhas abaixo dos dados
</commit_message>
<xml_diff>
--- a/planilha_de_gestor.xlsx
+++ b/planilha_de_gestor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williansantos/Documents/automacao_planilha/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williansantos/Documents/projetos-pessoais/automacao_planilha/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308E0E16-24D7-7A4D-837E-86D6FEF3AE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEC35A2-9291-914D-9ADE-5D0F8663872E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="106">
   <si>
     <t>Nº</t>
   </si>
@@ -369,18 +369,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -395,13 +389,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +612,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC40"/>
+  <dimension ref="A1:AC115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2377,9 +2369,3381 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:29" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="U40" s="5"/>
-      <c r="V40" s="5"/>
+    <row r="40" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="1">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1">
+        <v>10</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S40" s="1">
+        <v>1461</v>
+      </c>
+      <c r="T40" s="1">
+        <v>142035</v>
+      </c>
+      <c r="U40" s="2">
+        <v>45717.410416666666</v>
+      </c>
+      <c r="V40" s="2">
+        <v>45717.535416666666</v>
+      </c>
+      <c r="W40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="1">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1">
+        <v>10</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S41" s="1">
+        <v>3160</v>
+      </c>
+      <c r="T41" s="1">
+        <v>142037</v>
+      </c>
+      <c r="U41" s="2">
+        <v>45717.441666666666</v>
+      </c>
+      <c r="V41" s="2">
+        <v>45717.566666666666</v>
+      </c>
+      <c r="W41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC41" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="1">
+        <v>3</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1">
+        <v>10</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S42" s="1">
+        <v>3411</v>
+      </c>
+      <c r="T42" s="1">
+        <v>142061</v>
+      </c>
+      <c r="U42" s="2">
+        <v>45809.351388888892</v>
+      </c>
+      <c r="V42" s="2">
+        <v>45809.476388888892</v>
+      </c>
+      <c r="W42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC42" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="1">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1">
+        <v>10</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S43" s="1">
+        <v>1479</v>
+      </c>
+      <c r="T43" s="1">
+        <v>142112</v>
+      </c>
+      <c r="U43" s="2">
+        <v>45809.6875</v>
+      </c>
+      <c r="V43" s="2">
+        <v>45809.8125</v>
+      </c>
+      <c r="W43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC43" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="1">
+        <v>5</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1">
+        <v>10</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S44" s="1">
+        <v>3456</v>
+      </c>
+      <c r="T44" s="1">
+        <v>142121</v>
+      </c>
+      <c r="U44" s="2">
+        <v>45809.90625</v>
+      </c>
+      <c r="V44" s="2">
+        <v>45839.03125</v>
+      </c>
+      <c r="W44" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC44" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="1">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1">
+        <v>10</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S45" s="1">
+        <v>7299</v>
+      </c>
+      <c r="T45" s="1">
+        <v>142163</v>
+      </c>
+      <c r="U45" s="2">
+        <v>45839.802777777775</v>
+      </c>
+      <c r="V45" s="2">
+        <v>45839.09375</v>
+      </c>
+      <c r="W45" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC45" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="1">
+        <v>7</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1">
+        <v>10</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S46" s="1">
+        <v>5277</v>
+      </c>
+      <c r="T46" s="1">
+        <v>142172</v>
+      </c>
+      <c r="U46" s="2">
+        <v>45870.371527777781</v>
+      </c>
+      <c r="V46" s="2">
+        <v>45839.927777777775</v>
+      </c>
+      <c r="W46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC46" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="1">
+        <v>8</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1">
+        <v>10</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S47" s="1">
+        <v>4903</v>
+      </c>
+      <c r="T47" s="1">
+        <v>142212</v>
+      </c>
+      <c r="U47" s="2">
+        <v>45901.325694444444</v>
+      </c>
+      <c r="V47" s="2">
+        <v>45870.496527777781</v>
+      </c>
+      <c r="W47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC47" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="1">
+        <v>9</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1">
+        <v>10</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S48" s="1">
+        <v>2823</v>
+      </c>
+      <c r="T48" s="1">
+        <v>142229</v>
+      </c>
+      <c r="U48" s="2">
+        <v>45901.609722222223</v>
+      </c>
+      <c r="V48" s="2">
+        <v>45870.621527777781</v>
+      </c>
+      <c r="W48" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC48" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="1">
+        <v>10</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1">
+        <v>10</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S49" s="1">
+        <v>6093</v>
+      </c>
+      <c r="T49" s="1">
+        <v>142284</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V49" s="2">
+        <v>45901.450694444444</v>
+      </c>
+      <c r="W49" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC49" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="1">
+        <v>11</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1">
+        <v>10</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S50" s="1">
+        <v>2752</v>
+      </c>
+      <c r="T50" s="1">
+        <v>142435</v>
+      </c>
+      <c r="U50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V50" s="2">
+        <v>45901.734722222223</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC50" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="1">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1">
+        <v>10</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S51" s="1">
+        <v>2394</v>
+      </c>
+      <c r="T51" s="1">
+        <v>142464</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W51" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC51" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="1">
+        <v>13</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1">
+        <v>10</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S52" s="1">
+        <v>932</v>
+      </c>
+      <c r="T52" s="1">
+        <v>142536</v>
+      </c>
+      <c r="U52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W52" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC52" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="1">
+        <v>14</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1">
+        <v>10</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S53" s="1">
+        <v>11332</v>
+      </c>
+      <c r="T53" s="1">
+        <v>142576</v>
+      </c>
+      <c r="U53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V53" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W53" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC53" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="1">
+        <v>15</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1">
+        <v>10</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S54" s="1">
+        <v>605</v>
+      </c>
+      <c r="T54" s="1">
+        <v>142587</v>
+      </c>
+      <c r="U54" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V54" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W54" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC54" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="1">
+        <v>16</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1">
+        <v>10</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T55" s="1">
+        <v>142739</v>
+      </c>
+      <c r="U55" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V55" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W55" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC55" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="1">
+        <v>17</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1">
+        <v>10</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S56" s="1">
+        <v>2802</v>
+      </c>
+      <c r="T56" s="1">
+        <v>142835</v>
+      </c>
+      <c r="U56" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V56" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W56" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC56" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="1">
+        <v>18</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1">
+        <v>10</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S57" s="1">
+        <v>2559</v>
+      </c>
+      <c r="T57" s="1">
+        <v>142922</v>
+      </c>
+      <c r="U57" s="2">
+        <v>45690.540972222225</v>
+      </c>
+      <c r="V57" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W57" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC57" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="1">
+        <v>19</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1">
+        <v>10</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S58" s="1">
+        <v>994</v>
+      </c>
+      <c r="T58" s="1">
+        <v>143217</v>
+      </c>
+      <c r="U58" s="2">
+        <v>45749.671527777777</v>
+      </c>
+      <c r="V58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W58" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC58" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="1">
+        <v>20</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1">
+        <v>10</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S59" s="1">
+        <v>2152</v>
+      </c>
+      <c r="T59" s="1">
+        <v>143331</v>
+      </c>
+      <c r="U59" s="2">
+        <v>45840.38958333333</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W59" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC59" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="1">
+        <v>21</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1">
+        <v>10</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S60" s="1">
+        <v>4350</v>
+      </c>
+      <c r="T60" s="1">
+        <v>143429</v>
+      </c>
+      <c r="U60" s="2">
+        <v>45840.417361111111</v>
+      </c>
+      <c r="V60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W60" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC60" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="1">
+        <v>22</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1">
+        <v>10</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S61" s="1">
+        <v>6307</v>
+      </c>
+      <c r="T61" s="1">
+        <v>143502</v>
+      </c>
+      <c r="U61" s="2">
+        <v>45840.465277777781</v>
+      </c>
+      <c r="V61" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W61" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC61" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="1">
+        <v>23</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1">
+        <v>10</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R62" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S62" s="1">
+        <v>465</v>
+      </c>
+      <c r="T62" s="1">
+        <v>143757</v>
+      </c>
+      <c r="U62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="V62" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W62" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC62" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="1">
+        <v>24</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1">
+        <v>10</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S63" s="1">
+        <v>3381</v>
+      </c>
+      <c r="T63" s="1">
+        <v>144195</v>
+      </c>
+      <c r="U63" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V63" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W63" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC63" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="1">
+        <v>25</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1">
+        <v>10</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S64" s="1">
+        <v>520</v>
+      </c>
+      <c r="T64" s="1">
+        <v>144370</v>
+      </c>
+      <c r="U64" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V64" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W64" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC64" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="1">
+        <v>26</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1">
+        <v>10</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R65" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S65" s="1">
+        <v>945</v>
+      </c>
+      <c r="T65" s="1">
+        <v>144459</v>
+      </c>
+      <c r="U65" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="V65" s="2">
+        <v>45690.665972222225</v>
+      </c>
+      <c r="W65" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC65" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="1">
+        <v>27</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1">
+        <v>9</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S66" s="1">
+        <v>8004</v>
+      </c>
+      <c r="T66" s="1">
+        <v>142122</v>
+      </c>
+      <c r="U66" s="2">
+        <v>45809.96875</v>
+      </c>
+      <c r="V66" s="2">
+        <v>45718.777777777781</v>
+      </c>
+      <c r="W66" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC66" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="1">
+        <v>28</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1">
+        <v>9</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S67" s="1">
+        <v>6031</v>
+      </c>
+      <c r="T67" s="1">
+        <v>142467</v>
+      </c>
+      <c r="U67" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V67" s="2">
+        <v>45749.796527777777</v>
+      </c>
+      <c r="W67" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC67" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="1">
+        <v>29</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1">
+        <v>9</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R68" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S68" s="1">
+        <v>2858</v>
+      </c>
+      <c r="T68" s="1">
+        <v>142481</v>
+      </c>
+      <c r="U68" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="V68" s="2">
+        <v>45840.479861111111</v>
+      </c>
+      <c r="W68" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC68" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="1">
+        <v>30</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1">
+        <v>9</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R69" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S69" s="1">
+        <v>2596</v>
+      </c>
+      <c r="T69" s="1">
+        <v>142522</v>
+      </c>
+      <c r="U69" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V69" s="2">
+        <v>45840.51458333333</v>
+      </c>
+      <c r="W69" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC69" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="1">
+        <v>31</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1">
+        <v>9</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S70" s="1">
+        <v>2310</v>
+      </c>
+      <c r="T70" s="1">
+        <v>142560</v>
+      </c>
+      <c r="U70" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="V70" s="2">
+        <v>45840.518750000003</v>
+      </c>
+      <c r="W70" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC70" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="1">
+        <v>32</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1">
+        <v>9</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S71" s="1">
+        <v>5433</v>
+      </c>
+      <c r="T71" s="1">
+        <v>142569</v>
+      </c>
+      <c r="U71" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="V71" s="2">
+        <v>45840.542361111111</v>
+      </c>
+      <c r="W71" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC71" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="1">
+        <v>33</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1">
+        <v>9</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S72" s="1">
+        <v>601</v>
+      </c>
+      <c r="T72" s="1">
+        <v>142588</v>
+      </c>
+      <c r="U72" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="V72" s="2">
+        <v>45840.590277777781</v>
+      </c>
+      <c r="W72" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC72" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="1">
+        <v>34</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1">
+        <v>8</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R73" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S73" s="1">
+        <v>1750</v>
+      </c>
+      <c r="T73" s="1">
+        <v>142186</v>
+      </c>
+      <c r="U73" s="2">
+        <v>45870.496527777781</v>
+      </c>
+      <c r="V73" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="W73" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC73" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="1">
+        <v>35</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1">
+        <v>8</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S74" s="1">
+        <v>975</v>
+      </c>
+      <c r="T74" s="1">
+        <v>143105</v>
+      </c>
+      <c r="U74" s="2">
+        <v>45718.652777777781</v>
+      </c>
+      <c r="V74" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W74" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC74" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="1">
+        <v>36</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1">
+        <v>8</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S75" s="1">
+        <v>1023</v>
+      </c>
+      <c r="T75" s="1">
+        <v>143327</v>
+      </c>
+      <c r="U75" s="2">
+        <v>45840.354861111111</v>
+      </c>
+      <c r="V75" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="W75" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC75" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="1">
+        <v>37</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1">
+        <v>8</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R76" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S76" s="1">
+        <v>1926</v>
+      </c>
+      <c r="T76" s="1">
+        <v>143333</v>
+      </c>
+      <c r="U76" s="2">
+        <v>45840.393750000003</v>
+      </c>
+      <c r="V76" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="W76" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC76" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="1">
+        <v>38</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1">
+        <v>8</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S77" s="1">
+        <v>11594</v>
+      </c>
+      <c r="T77" s="1">
+        <v>144129</v>
+      </c>
+      <c r="U77" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="V77" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W77" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC77" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="1">
+        <v>1</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1">
+        <v>10</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S78" s="1">
+        <v>1461</v>
+      </c>
+      <c r="T78" s="1">
+        <v>142035</v>
+      </c>
+      <c r="U78" s="2">
+        <v>45717.410416666666</v>
+      </c>
+      <c r="V78" s="2">
+        <v>45717.535416666666</v>
+      </c>
+      <c r="W78" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC78" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="1">
+        <v>2</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1">
+        <v>10</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R79" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S79" s="1">
+        <v>3160</v>
+      </c>
+      <c r="T79" s="1">
+        <v>142037</v>
+      </c>
+      <c r="U79" s="2">
+        <v>45717.441666666666</v>
+      </c>
+      <c r="V79" s="2">
+        <v>45717.566666666666</v>
+      </c>
+      <c r="W79" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC79" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="1">
+        <v>3</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1">
+        <v>10</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R80" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S80" s="1">
+        <v>3411</v>
+      </c>
+      <c r="T80" s="1">
+        <v>142061</v>
+      </c>
+      <c r="U80" s="2">
+        <v>45809.351388888892</v>
+      </c>
+      <c r="V80" s="2">
+        <v>45809.476388888892</v>
+      </c>
+      <c r="W80" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC80" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="1">
+        <v>4</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1">
+        <v>10</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S81" s="1">
+        <v>1479</v>
+      </c>
+      <c r="T81" s="1">
+        <v>142112</v>
+      </c>
+      <c r="U81" s="2">
+        <v>45809.6875</v>
+      </c>
+      <c r="V81" s="2">
+        <v>45809.8125</v>
+      </c>
+      <c r="W81" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC81" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="1">
+        <v>5</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1">
+        <v>10</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S82" s="1">
+        <v>3456</v>
+      </c>
+      <c r="T82" s="1">
+        <v>142121</v>
+      </c>
+      <c r="U82" s="2">
+        <v>45809.90625</v>
+      </c>
+      <c r="V82" s="2">
+        <v>45839.03125</v>
+      </c>
+      <c r="W82" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC82" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="1">
+        <v>6</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1">
+        <v>10</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S83" s="1">
+        <v>7299</v>
+      </c>
+      <c r="T83" s="1">
+        <v>142163</v>
+      </c>
+      <c r="U83" s="2">
+        <v>45839.802777777775</v>
+      </c>
+      <c r="V83" s="2">
+        <v>45839.09375</v>
+      </c>
+      <c r="W83" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC83" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="1">
+        <v>7</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1">
+        <v>10</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S84" s="1">
+        <v>5277</v>
+      </c>
+      <c r="T84" s="1">
+        <v>142172</v>
+      </c>
+      <c r="U84" s="2">
+        <v>45870.371527777781</v>
+      </c>
+      <c r="V84" s="2">
+        <v>45839.927777777775</v>
+      </c>
+      <c r="W84" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC84" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="1">
+        <v>8</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1">
+        <v>10</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S85" s="1">
+        <v>4903</v>
+      </c>
+      <c r="T85" s="1">
+        <v>142212</v>
+      </c>
+      <c r="U85" s="2">
+        <v>45901.325694444444</v>
+      </c>
+      <c r="V85" s="2">
+        <v>45870.496527777781</v>
+      </c>
+      <c r="W85" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC85" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="1">
+        <v>9</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1">
+        <v>10</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S86" s="1">
+        <v>2823</v>
+      </c>
+      <c r="T86" s="1">
+        <v>142229</v>
+      </c>
+      <c r="U86" s="2">
+        <v>45901.609722222223</v>
+      </c>
+      <c r="V86" s="2">
+        <v>45870.621527777781</v>
+      </c>
+      <c r="W86" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC86" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="1">
+        <v>10</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1">
+        <v>10</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L87" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S87" s="1">
+        <v>6093</v>
+      </c>
+      <c r="T87" s="1">
+        <v>142284</v>
+      </c>
+      <c r="U87" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V87" s="2">
+        <v>45901.450694444444</v>
+      </c>
+      <c r="W87" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC87" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="1">
+        <v>11</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1">
+        <v>10</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L88" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S88" s="1">
+        <v>2752</v>
+      </c>
+      <c r="T88" s="1">
+        <v>142435</v>
+      </c>
+      <c r="U88" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V88" s="2">
+        <v>45901.734722222223</v>
+      </c>
+      <c r="W88" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC88" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="1">
+        <v>12</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1">
+        <v>10</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R89" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S89" s="1">
+        <v>2394</v>
+      </c>
+      <c r="T89" s="1">
+        <v>142464</v>
+      </c>
+      <c r="U89" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V89" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W89" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC89" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="1">
+        <v>13</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1">
+        <v>10</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L90" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S90" s="1">
+        <v>932</v>
+      </c>
+      <c r="T90" s="1">
+        <v>142536</v>
+      </c>
+      <c r="U90" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V90" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W90" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC90" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="1">
+        <v>14</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1">
+        <v>10</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R91" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S91" s="1">
+        <v>11332</v>
+      </c>
+      <c r="T91" s="1">
+        <v>142576</v>
+      </c>
+      <c r="U91" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V91" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W91" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC91" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="1">
+        <v>15</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1">
+        <v>10</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R92" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S92" s="1">
+        <v>605</v>
+      </c>
+      <c r="T92" s="1">
+        <v>142587</v>
+      </c>
+      <c r="U92" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V92" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W92" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC92" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="1">
+        <v>16</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1">
+        <v>10</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R93" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T93" s="1">
+        <v>142739</v>
+      </c>
+      <c r="U93" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V93" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W93" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC93" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="1">
+        <v>17</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1">
+        <v>10</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L94" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S94" s="1">
+        <v>2802</v>
+      </c>
+      <c r="T94" s="1">
+        <v>142835</v>
+      </c>
+      <c r="U94" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V94" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W94" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC94" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="1">
+        <v>18</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1">
+        <v>10</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L95" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S95" s="1">
+        <v>2559</v>
+      </c>
+      <c r="T95" s="1">
+        <v>142922</v>
+      </c>
+      <c r="U95" s="2">
+        <v>45690.540972222225</v>
+      </c>
+      <c r="V95" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W95" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC95" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="1">
+        <v>19</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1">
+        <v>10</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R96" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S96" s="1">
+        <v>994</v>
+      </c>
+      <c r="T96" s="1">
+        <v>143217</v>
+      </c>
+      <c r="U96" s="2">
+        <v>45749.671527777777</v>
+      </c>
+      <c r="V96" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W96" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC96" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="1">
+        <v>20</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1">
+        <v>10</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N97" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R97" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S97" s="1">
+        <v>2152</v>
+      </c>
+      <c r="T97" s="1">
+        <v>143331</v>
+      </c>
+      <c r="U97" s="2">
+        <v>45840.38958333333</v>
+      </c>
+      <c r="V97" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W97" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC97" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="1">
+        <v>21</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1">
+        <v>10</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N98" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R98" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S98" s="1">
+        <v>4350</v>
+      </c>
+      <c r="T98" s="1">
+        <v>143429</v>
+      </c>
+      <c r="U98" s="2">
+        <v>45840.417361111111</v>
+      </c>
+      <c r="V98" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W98" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC98" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="1">
+        <v>22</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1">
+        <v>10</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P99" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R99" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S99" s="1">
+        <v>6307</v>
+      </c>
+      <c r="T99" s="1">
+        <v>143502</v>
+      </c>
+      <c r="U99" s="2">
+        <v>45840.465277777781</v>
+      </c>
+      <c r="V99" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W99" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC99" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="1">
+        <v>23</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1">
+        <v>10</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L100" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M100" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R100" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S100" s="1">
+        <v>465</v>
+      </c>
+      <c r="T100" s="1">
+        <v>143757</v>
+      </c>
+      <c r="U100" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="V100" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W100" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC100" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="101" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="1">
+        <v>24</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1">
+        <v>10</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M101" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R101" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S101" s="1">
+        <v>3381</v>
+      </c>
+      <c r="T101" s="1">
+        <v>144195</v>
+      </c>
+      <c r="U101" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V101" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W101" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC101" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="1">
+        <v>25</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1">
+        <v>10</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M102" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S102" s="1">
+        <v>520</v>
+      </c>
+      <c r="T102" s="1">
+        <v>144370</v>
+      </c>
+      <c r="U102" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V102" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W102" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC102" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="1">
+        <v>26</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1">
+        <v>10</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N103" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R103" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S103" s="1">
+        <v>945</v>
+      </c>
+      <c r="T103" s="1">
+        <v>144459</v>
+      </c>
+      <c r="U103" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="V103" s="2">
+        <v>45690.665972222225</v>
+      </c>
+      <c r="W103" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC103" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="104" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="1">
+        <v>27</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1">
+        <v>9</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R104" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S104" s="1">
+        <v>8004</v>
+      </c>
+      <c r="T104" s="1">
+        <v>142122</v>
+      </c>
+      <c r="U104" s="2">
+        <v>45809.96875</v>
+      </c>
+      <c r="V104" s="2">
+        <v>45718.777777777781</v>
+      </c>
+      <c r="W104" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC104" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="1">
+        <v>28</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1">
+        <v>9</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R105" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S105" s="1">
+        <v>6031</v>
+      </c>
+      <c r="T105" s="1">
+        <v>142467</v>
+      </c>
+      <c r="U105" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V105" s="2">
+        <v>45749.796527777777</v>
+      </c>
+      <c r="W105" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC105" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A106" s="1">
+        <v>29</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1">
+        <v>9</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L106" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N106" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R106" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S106" s="1">
+        <v>2858</v>
+      </c>
+      <c r="T106" s="1">
+        <v>142481</v>
+      </c>
+      <c r="U106" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="V106" s="2">
+        <v>45840.479861111111</v>
+      </c>
+      <c r="W106" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC106" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A107" s="1">
+        <v>30</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1">
+        <v>9</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L107" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R107" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S107" s="1">
+        <v>2596</v>
+      </c>
+      <c r="T107" s="1">
+        <v>142522</v>
+      </c>
+      <c r="U107" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V107" s="2">
+        <v>45840.51458333333</v>
+      </c>
+      <c r="W107" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC107" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="1">
+        <v>31</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1">
+        <v>9</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N108" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q108" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S108" s="1">
+        <v>2310</v>
+      </c>
+      <c r="T108" s="1">
+        <v>142560</v>
+      </c>
+      <c r="U108" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="V108" s="2">
+        <v>45840.518750000003</v>
+      </c>
+      <c r="W108" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC108" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A109" s="1">
+        <v>32</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1">
+        <v>9</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S109" s="1">
+        <v>5433</v>
+      </c>
+      <c r="T109" s="1">
+        <v>142569</v>
+      </c>
+      <c r="U109" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="V109" s="2">
+        <v>45840.542361111111</v>
+      </c>
+      <c r="W109" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC109" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A110" s="1">
+        <v>33</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1">
+        <v>9</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L110" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R110" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S110" s="1">
+        <v>601</v>
+      </c>
+      <c r="T110" s="1">
+        <v>142588</v>
+      </c>
+      <c r="U110" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="V110" s="2">
+        <v>45840.590277777781</v>
+      </c>
+      <c r="W110" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC110" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="111" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A111" s="1">
+        <v>34</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1">
+        <v>8</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L111" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R111" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S111" s="1">
+        <v>1750</v>
+      </c>
+      <c r="T111" s="1">
+        <v>142186</v>
+      </c>
+      <c r="U111" s="2">
+        <v>45870.496527777781</v>
+      </c>
+      <c r="V111" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="W111" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC111" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A112" s="1">
+        <v>35</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1">
+        <v>8</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M112" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S112" s="1">
+        <v>975</v>
+      </c>
+      <c r="T112" s="1">
+        <v>143105</v>
+      </c>
+      <c r="U112" s="2">
+        <v>45718.652777777781</v>
+      </c>
+      <c r="V112" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W112" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC112" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A113" s="1">
+        <v>36</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1">
+        <v>8</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M113" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P113" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S113" s="1">
+        <v>1023</v>
+      </c>
+      <c r="T113" s="1">
+        <v>143327</v>
+      </c>
+      <c r="U113" s="2">
+        <v>45840.354861111111</v>
+      </c>
+      <c r="V113" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="W113" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC113" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="114" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A114" s="1">
+        <v>37</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1">
+        <v>8</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R114" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S114" s="1">
+        <v>1926</v>
+      </c>
+      <c r="T114" s="1">
+        <v>143333</v>
+      </c>
+      <c r="U114" s="2">
+        <v>45840.393750000003</v>
+      </c>
+      <c r="V114" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="W114" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC114" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A115" s="1">
+        <v>38</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1">
+        <v>8</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L115" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S115" s="1">
+        <v>11594</v>
+      </c>
+      <c r="T115" s="1">
+        <v>144129</v>
+      </c>
+      <c r="U115" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="V115" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W115" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC115" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2421,6 +5785,82 @@
     <hyperlink ref="W37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="W38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="W39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="W40" r:id="rId39" xr:uid="{110741DD-D5F6-5542-A02C-A3D0A90405EB}"/>
+    <hyperlink ref="W41" r:id="rId40" xr:uid="{53E09F93-65CB-3449-8222-81831BC99FD3}"/>
+    <hyperlink ref="W42" r:id="rId41" xr:uid="{B46C91C8-0737-264C-82BC-DE81CA674297}"/>
+    <hyperlink ref="W43" r:id="rId42" xr:uid="{10759CB5-561A-2B48-AC65-4300808C4BC3}"/>
+    <hyperlink ref="W44" r:id="rId43" xr:uid="{1B46D277-6270-D848-98C1-3CDAA43C736B}"/>
+    <hyperlink ref="W45" r:id="rId44" xr:uid="{C33D239D-6EAF-5944-A6CA-AF110801A9A4}"/>
+    <hyperlink ref="W46" r:id="rId45" xr:uid="{C7F6A741-965D-7342-AF40-8D1B51665BDC}"/>
+    <hyperlink ref="W47" r:id="rId46" xr:uid="{925CABB1-F6A5-8D43-BCAE-949453AFF75E}"/>
+    <hyperlink ref="W48" r:id="rId47" xr:uid="{D3504C04-8499-9243-8407-B336618E7C7C}"/>
+    <hyperlink ref="W49" r:id="rId48" xr:uid="{3D5C1A15-6D87-4A49-86C6-58079DDD813D}"/>
+    <hyperlink ref="W50" r:id="rId49" xr:uid="{9133732F-8A4C-2346-957D-C9E72FCFD3D9}"/>
+    <hyperlink ref="W51" r:id="rId50" xr:uid="{AE033A9A-ACFD-E942-A666-2855143CCAE0}"/>
+    <hyperlink ref="W52" r:id="rId51" xr:uid="{E7702DE6-A7CF-0F49-8F73-842B371940AB}"/>
+    <hyperlink ref="W53" r:id="rId52" xr:uid="{69037754-49A5-3848-94ED-6644F13BDBD9}"/>
+    <hyperlink ref="W54" r:id="rId53" xr:uid="{1A93835A-A81B-884B-AA40-9C18BC4B2DC0}"/>
+    <hyperlink ref="W55" r:id="rId54" xr:uid="{EE26CA5D-9216-DB46-8106-87D47ECDE017}"/>
+    <hyperlink ref="W56" r:id="rId55" xr:uid="{DBDA709E-EDFB-5746-9A85-19104B35A0AA}"/>
+    <hyperlink ref="W57" r:id="rId56" xr:uid="{46D70798-E3D4-1B42-9C41-5B6FBFCAFFDD}"/>
+    <hyperlink ref="W58" r:id="rId57" xr:uid="{587DAAFC-4450-7C41-878C-140C583C3D53}"/>
+    <hyperlink ref="W59" r:id="rId58" xr:uid="{097268B4-996B-C743-97A3-EBC1B0717A43}"/>
+    <hyperlink ref="W60" r:id="rId59" xr:uid="{C181CE63-05B7-8145-9786-60502F5CECF1}"/>
+    <hyperlink ref="W61" r:id="rId60" xr:uid="{2373C319-E81F-0A4E-A972-10784FD66924}"/>
+    <hyperlink ref="W62" r:id="rId61" xr:uid="{EBBB8813-2959-7243-9526-E24EA862A4B7}"/>
+    <hyperlink ref="W63" r:id="rId62" xr:uid="{B1238720-1478-8C4C-926F-00CB6B107E8C}"/>
+    <hyperlink ref="W64" r:id="rId63" xr:uid="{46207364-7D69-E645-A378-EB14540F0070}"/>
+    <hyperlink ref="W65" r:id="rId64" xr:uid="{F7C34490-14B5-2946-A7DC-9A73F57AEC87}"/>
+    <hyperlink ref="W66" r:id="rId65" xr:uid="{9281E64C-FADD-AC45-81F0-E86AE9274E58}"/>
+    <hyperlink ref="W67" r:id="rId66" xr:uid="{7F443A34-6220-A341-AEED-3691F8CB8220}"/>
+    <hyperlink ref="W68" r:id="rId67" xr:uid="{AD22E289-D281-0343-A46F-F9A561972B6E}"/>
+    <hyperlink ref="W69" r:id="rId68" xr:uid="{D9685A9D-63F9-434F-8FF6-8F0E397F1A04}"/>
+    <hyperlink ref="W70" r:id="rId69" xr:uid="{DD7C65EE-906D-014B-89BE-E834B952B2BD}"/>
+    <hyperlink ref="W71" r:id="rId70" xr:uid="{0DD44177-E64F-084D-90A3-6ED87D38472B}"/>
+    <hyperlink ref="W72" r:id="rId71" xr:uid="{76316631-2932-BA42-94D4-C36ECE0E6712}"/>
+    <hyperlink ref="W73" r:id="rId72" xr:uid="{6E80A4D5-D61E-9C49-8771-20AFA2A15A62}"/>
+    <hyperlink ref="W74" r:id="rId73" xr:uid="{15DB4CFA-038E-2B47-BAA7-791D38206998}"/>
+    <hyperlink ref="W75" r:id="rId74" xr:uid="{7779C5A2-723A-C044-8ACC-3F30D2E5BB41}"/>
+    <hyperlink ref="W76" r:id="rId75" xr:uid="{D4F999C7-1B0E-4243-98D0-90272491E797}"/>
+    <hyperlink ref="W77" r:id="rId76" xr:uid="{3B97D579-8A5B-CF4C-A3C0-1BA1F35A5649}"/>
+    <hyperlink ref="W78" r:id="rId77" xr:uid="{8FB4C4C3-3158-C744-99F1-C2F7C9C0AA44}"/>
+    <hyperlink ref="W79" r:id="rId78" xr:uid="{179B3316-220F-AD4C-A5BC-D65538195225}"/>
+    <hyperlink ref="W80" r:id="rId79" xr:uid="{89183D13-E525-BF4B-9A19-2B6EB9CE6339}"/>
+    <hyperlink ref="W81" r:id="rId80" xr:uid="{4BC63230-07FD-E348-A117-B32189B1699D}"/>
+    <hyperlink ref="W82" r:id="rId81" xr:uid="{26B21CBB-6EFB-9843-8307-FAC4A1CF9D92}"/>
+    <hyperlink ref="W83" r:id="rId82" xr:uid="{E9EF81FE-0E85-0246-8939-18D548CC1154}"/>
+    <hyperlink ref="W84" r:id="rId83" xr:uid="{60FEC5C8-0213-6F41-9BCE-36090D088EFB}"/>
+    <hyperlink ref="W85" r:id="rId84" xr:uid="{5E62893F-DCAE-9949-8F1B-143534F44004}"/>
+    <hyperlink ref="W86" r:id="rId85" xr:uid="{428E4C40-D6D4-A840-87B4-80C58A96CDF0}"/>
+    <hyperlink ref="W87" r:id="rId86" xr:uid="{F2C03E36-B2B2-2F40-97F0-759CC4769114}"/>
+    <hyperlink ref="W88" r:id="rId87" xr:uid="{018B0A86-2464-1442-9502-5DD1BD191F39}"/>
+    <hyperlink ref="W89" r:id="rId88" xr:uid="{FD81BCB7-19D7-524C-9F16-1DB80DF239C0}"/>
+    <hyperlink ref="W90" r:id="rId89" xr:uid="{C516700A-EF62-3342-A74E-CE21A72DEFC2}"/>
+    <hyperlink ref="W91" r:id="rId90" xr:uid="{E7F423B2-911B-E245-BC36-B312BA95849F}"/>
+    <hyperlink ref="W92" r:id="rId91" xr:uid="{FF69D647-251C-3D43-876D-DA283BEDE8F6}"/>
+    <hyperlink ref="W93" r:id="rId92" xr:uid="{F6B8B091-82D3-A345-A0C2-507336254960}"/>
+    <hyperlink ref="W94" r:id="rId93" xr:uid="{7DEC1B80-AA49-B840-A2DC-4AD9F7081E1C}"/>
+    <hyperlink ref="W95" r:id="rId94" xr:uid="{63B1CAC1-85D8-3045-A76B-62A68BAC21CD}"/>
+    <hyperlink ref="W96" r:id="rId95" xr:uid="{4408550F-485E-6B4C-8187-8D5F7FA48E0E}"/>
+    <hyperlink ref="W97" r:id="rId96" xr:uid="{E56B82DE-586D-194A-BE4D-1FB39E9DF847}"/>
+    <hyperlink ref="W98" r:id="rId97" xr:uid="{3A9DA92F-41E8-5944-AB5D-966E84B965BF}"/>
+    <hyperlink ref="W99" r:id="rId98" xr:uid="{8193D04A-9050-0746-A67C-C0B8B118BD90}"/>
+    <hyperlink ref="W100" r:id="rId99" xr:uid="{4370B43F-D114-1A4C-828E-7CA782766F7A}"/>
+    <hyperlink ref="W101" r:id="rId100" xr:uid="{E7F8503B-6C93-0449-8BA2-CC98CF8FE5FD}"/>
+    <hyperlink ref="W102" r:id="rId101" xr:uid="{ACC0375D-3333-4144-A1C3-516825106D89}"/>
+    <hyperlink ref="W103" r:id="rId102" xr:uid="{19750E66-85F0-4947-9343-DA7FB84E43A7}"/>
+    <hyperlink ref="W104" r:id="rId103" xr:uid="{021CE917-799D-D945-9C6C-295BFECC7F47}"/>
+    <hyperlink ref="W105" r:id="rId104" xr:uid="{8F188E73-D166-7D41-BFDC-17D38D49DC50}"/>
+    <hyperlink ref="W106" r:id="rId105" xr:uid="{F18BD781-F284-754E-BE8F-A96159F7B95F}"/>
+    <hyperlink ref="W107" r:id="rId106" xr:uid="{2AD57D58-2FD3-5049-9701-65BE8413F9A1}"/>
+    <hyperlink ref="W108" r:id="rId107" xr:uid="{300A7B8C-7183-7A49-A198-1983165FFDD6}"/>
+    <hyperlink ref="W109" r:id="rId108" xr:uid="{E3B7DDFD-D822-494D-B4BB-F39008D7052C}"/>
+    <hyperlink ref="W110" r:id="rId109" xr:uid="{00C15B3E-97B8-274E-AEEA-790372990347}"/>
+    <hyperlink ref="W111" r:id="rId110" xr:uid="{908CB990-1C59-6F4E-98C3-0F4B5B2793DD}"/>
+    <hyperlink ref="W112" r:id="rId111" xr:uid="{D18BC39B-A5AE-F646-BE71-5D8D62E87289}"/>
+    <hyperlink ref="W113" r:id="rId112" xr:uid="{6D41150D-38B0-C24A-B0BB-10CE151B62AA}"/>
+    <hyperlink ref="W114" r:id="rId113" xr:uid="{7BE9E7CD-B062-8144-A896-AFF09089C621}"/>
+    <hyperlink ref="W115" r:id="rId114" xr:uid="{0C729F24-D240-C146-8E93-7723504852DC}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>